<commit_message>
slovenia and germany focus tree things
</commit_message>
<xml_diff>
--- a/plans/Germany Focus Tree.xlsx
+++ b/plans/Germany Focus Tree.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
@@ -18,10 +18,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Author</author>
+    <author>Forfatter</author>
   </authors>
   <commentList>
-    <comment ref="F3" authorId="0">
+    <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -31,7 +31,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Author:</t>
+          <t>Forfatter:</t>
         </r>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0">
+    <comment ref="D4" authorId="0" shapeId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Author:</t>
+          <t>Forfatter:</t>
         </r>
         <r>
           <rPr>
@@ -69,12 +69,36 @@
         </r>
       </text>
     </comment>
+    <comment ref="Z6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Gives a "Landkreuzer" division with a special unit</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="231" uniqueCount="174">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="179">
   <si>
     <t>Illyria  Parties</t>
   </si>
@@ -556,9 +580,6 @@
     <t>Foreign Volunteer Divisions</t>
   </si>
   <si>
-    <t>Expand the SS Army</t>
-  </si>
-  <si>
     <t>The German War Machine</t>
   </si>
   <si>
@@ -574,18 +595,9 @@
     <t>Goebbels' Administration</t>
   </si>
   <si>
-    <t>Motorized Transports</t>
-  </si>
-  <si>
     <t>Establish the Volkssturm</t>
   </si>
   <si>
-    <t>A Noble Army</t>
-  </si>
-  <si>
-    <t>Discredit Communism</t>
-  </si>
-  <si>
     <t>Mobile Warfare</t>
   </si>
   <si>
@@ -596,12 +608,39 @@
   </si>
   <si>
     <t>Armor Innovations</t>
+  </si>
+  <si>
+    <t>The Noble Army</t>
+  </si>
+  <si>
+    <t>Battle Against Communism</t>
+  </si>
+  <si>
+    <t>Form the SS Army</t>
+  </si>
+  <si>
+    <t>Expand the Military Police</t>
+  </si>
+  <si>
+    <t>Allow Foreigners to Join</t>
+  </si>
+  <si>
+    <t>Compulsive Service for the Occupied</t>
+  </si>
+  <si>
+    <t>SS Cavalry Brigades</t>
+  </si>
+  <si>
+    <t>Panzergrenadiers</t>
+  </si>
+  <si>
+    <t>SP Artillery</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -786,7 +825,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -795,27 +840,21 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -833,7 +872,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -875,7 +914,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -908,9 +947,26 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -943,6 +999,23 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1121,11 +1194,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AB12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q4" sqref="Q4:R4"/>
+    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
+      <selection activeCell="AF2" sqref="AF2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="7.140625" style="1"/>
   </cols>
@@ -1134,265 +1207,275 @@
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="21" t="s">
+      <c r="D1" s="28" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="21"/>
+      <c r="E1" s="28"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
-      <c r="V1" s="24" t="s">
+      <c r="V1" s="22" t="s">
         <v>157</v>
       </c>
-      <c r="W1" s="24"/>
+      <c r="W1" s="22"/>
     </row>
     <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="22" t="s">
+      <c r="C2" s="24" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="22"/>
-      <c r="E2" s="22" t="s">
+      <c r="D2" s="24"/>
+      <c r="E2" s="24" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="22"/>
+      <c r="F2" s="24"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="27" t="s">
+      <c r="I2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="27"/>
-      <c r="R2" s="24" t="s">
+      <c r="J2" s="29"/>
+      <c r="R2" s="22" t="s">
         <v>147</v>
       </c>
-      <c r="S2" s="24"/>
-      <c r="V2" s="24" t="s">
+      <c r="S2" s="22"/>
+      <c r="V2" s="22" t="s">
+        <v>172</v>
+      </c>
+      <c r="W2" s="22"/>
+      <c r="Z2" s="22" t="s">
         <v>160</v>
       </c>
-      <c r="W2" s="24"/>
-      <c r="Z2" s="24" t="s">
-        <v>161</v>
-      </c>
-      <c r="AA2" s="24"/>
+      <c r="AA2" s="22"/>
     </row>
     <row r="3" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="26" t="s">
+      <c r="B3" s="23" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="26"/>
-      <c r="D3" s="26" t="s">
+      <c r="C3" s="23"/>
+      <c r="D3" s="23" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="26"/>
-      <c r="F3" s="26" t="s">
+      <c r="E3" s="23"/>
+      <c r="F3" s="23" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="26"/>
+      <c r="G3" s="23"/>
       <c r="H3" s="20"/>
-      <c r="L3" s="21" t="s">
+      <c r="L3" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="21"/>
-      <c r="Q3" s="25" t="s">
+      <c r="M3" s="28"/>
+      <c r="Q3" s="27" t="s">
         <v>148</v>
       </c>
-      <c r="R3" s="25"/>
-      <c r="S3" s="25" t="s">
+      <c r="R3" s="27"/>
+      <c r="S3" s="27" t="s">
         <v>154</v>
       </c>
-      <c r="T3" s="25"/>
-      <c r="U3" s="23" t="s">
+      <c r="T3" s="27"/>
+      <c r="U3" s="25" t="s">
         <v>158</v>
       </c>
-      <c r="V3" s="23"/>
-      <c r="W3" s="23" t="s">
+      <c r="V3" s="25"/>
+      <c r="W3" s="25" t="s">
+        <v>174</v>
+      </c>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="23" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z3" s="23"/>
+      <c r="AA3" s="23" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB3" s="23"/>
+    </row>
+    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="28" t="s">
+        <v>125</v>
+      </c>
+      <c r="C4" s="28"/>
+      <c r="D4" s="22" t="s">
+        <v>145</v>
+      </c>
+      <c r="E4" s="22"/>
+      <c r="F4" s="28" t="s">
+        <v>156</v>
+      </c>
+      <c r="G4" s="28"/>
+      <c r="J4" s="22" t="s">
+        <v>134</v>
+      </c>
+      <c r="K4" s="22"/>
+      <c r="N4" s="26" t="s">
+        <v>138</v>
+      </c>
+      <c r="O4" s="26"/>
+      <c r="P4" s="21"/>
+      <c r="Q4" s="22" t="s">
+        <v>150</v>
+      </c>
+      <c r="R4" s="22"/>
+      <c r="S4" s="22" t="s">
+        <v>153</v>
+      </c>
+      <c r="T4" s="22"/>
+      <c r="U4" s="23" t="s">
+        <v>173</v>
+      </c>
+      <c r="V4" s="23"/>
+      <c r="W4" s="23" t="s">
+        <v>176</v>
+      </c>
+      <c r="X4" s="23"/>
+      <c r="Y4" s="24" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z4" s="24"/>
+      <c r="AA4" s="24" t="s">
+        <v>168</v>
+      </c>
+      <c r="AB4" s="24"/>
+    </row>
+    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="23"/>
+      <c r="C5" s="23" t="s">
+        <v>126</v>
+      </c>
+      <c r="D5" s="23"/>
+      <c r="E5" s="24" t="s">
+        <v>152</v>
+      </c>
+      <c r="F5" s="24"/>
+      <c r="G5" s="24" t="s">
+        <v>151</v>
+      </c>
+      <c r="H5" s="24"/>
+      <c r="J5" s="22" t="s">
+        <v>135</v>
+      </c>
+      <c r="K5" s="22"/>
+      <c r="N5" s="26" t="s">
+        <v>139</v>
+      </c>
+      <c r="O5" s="26"/>
+      <c r="P5" s="21"/>
+      <c r="Q5" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="R5" s="22"/>
+      <c r="S5" s="22" t="s">
+        <v>171</v>
+      </c>
+      <c r="T5" s="22"/>
+      <c r="U5" s="24" t="s">
+        <v>165</v>
+      </c>
+      <c r="V5" s="24"/>
+      <c r="W5" s="24" t="s">
         <v>159</v>
       </c>
-      <c r="X3" s="23"/>
-      <c r="Y3" s="26" t="s">
+      <c r="X5" s="24"/>
+      <c r="Y5" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="Z3" s="26"/>
-      <c r="AA3" s="26" t="s">
-        <v>171</v>
-      </c>
-      <c r="AB3" s="26"/>
-    </row>
-    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="21" t="s">
-        <v>125</v>
-      </c>
-      <c r="C4" s="21"/>
-      <c r="D4" s="24" t="s">
-        <v>145</v>
-      </c>
-      <c r="E4" s="24"/>
-      <c r="F4" s="21" t="s">
-        <v>156</v>
-      </c>
-      <c r="G4" s="21"/>
-      <c r="J4" s="24" t="s">
-        <v>134</v>
-      </c>
-      <c r="K4" s="24"/>
-      <c r="N4" s="28" t="s">
-        <v>138</v>
-      </c>
-      <c r="O4" s="28"/>
-      <c r="P4" s="29"/>
-      <c r="Q4" s="24" t="s">
-        <v>150</v>
-      </c>
-      <c r="R4" s="24"/>
-      <c r="S4" s="24" t="s">
-        <v>153</v>
-      </c>
-      <c r="T4" s="24"/>
-      <c r="U4" s="26"/>
-      <c r="V4" s="26"/>
-      <c r="W4" s="26"/>
-      <c r="X4" s="26"/>
-      <c r="Y4" s="22"/>
-      <c r="Z4" s="22"/>
-      <c r="AA4" s="22" t="s">
-        <v>172</v>
-      </c>
-      <c r="AB4" s="22"/>
-    </row>
-    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="B5" s="26"/>
-      <c r="C5" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="D5" s="26"/>
-      <c r="E5" s="22" t="s">
-        <v>152</v>
-      </c>
-      <c r="F5" s="22"/>
-      <c r="G5" s="22" t="s">
-        <v>151</v>
-      </c>
-      <c r="H5" s="22"/>
-      <c r="J5" s="24" t="s">
-        <v>135</v>
-      </c>
-      <c r="K5" s="24"/>
-      <c r="N5" s="28" t="s">
-        <v>139</v>
-      </c>
-      <c r="O5" s="28"/>
-      <c r="P5" s="29"/>
-      <c r="Q5" s="24" t="s">
-        <v>168</v>
-      </c>
-      <c r="R5" s="24"/>
-      <c r="S5" s="24" t="s">
+      <c r="Z5" s="23"/>
+      <c r="AA5" s="23" t="s">
         <v>169</v>
       </c>
-      <c r="T5" s="24"/>
-      <c r="U5" s="22" t="s">
-        <v>167</v>
-      </c>
-      <c r="V5" s="22"/>
-      <c r="W5" s="22"/>
-      <c r="X5" s="22"/>
-      <c r="Y5" s="26" t="s">
-        <v>170</v>
-      </c>
-      <c r="Z5" s="26"/>
-      <c r="AA5" s="26" t="s">
-        <v>173</v>
-      </c>
-      <c r="AB5" s="26"/>
+      <c r="AB5" s="23"/>
     </row>
     <row r="6" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="27" t="s">
+      <c r="D6" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="27"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="25" t="s">
+      <c r="I6" s="27" t="s">
         <v>136</v>
       </c>
-      <c r="J6" s="25"/>
-      <c r="K6" s="25" t="s">
+      <c r="J6" s="27"/>
+      <c r="K6" s="27" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="25"/>
-      <c r="M6" s="23" t="s">
+      <c r="L6" s="27"/>
+      <c r="M6" s="25" t="s">
         <v>140</v>
       </c>
-      <c r="N6" s="23"/>
-      <c r="O6" s="23" t="s">
+      <c r="N6" s="25"/>
+      <c r="O6" s="25" t="s">
         <v>141</v>
       </c>
-      <c r="P6" s="23"/>
-      <c r="R6" s="24" t="s">
+      <c r="P6" s="25"/>
+      <c r="R6" s="22" t="s">
         <v>149</v>
       </c>
-      <c r="S6" s="24"/>
-      <c r="V6" s="24"/>
-      <c r="W6" s="24"/>
-      <c r="Z6" s="24" t="s">
-        <v>162</v>
-      </c>
-      <c r="AA6" s="24"/>
+      <c r="S6" s="22"/>
+      <c r="V6" s="22" t="s">
+        <v>175</v>
+      </c>
+      <c r="W6" s="22"/>
+      <c r="Z6" s="22" t="s">
+        <v>161</v>
+      </c>
+      <c r="AA6" s="22"/>
     </row>
     <row r="7" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A7" s="24" t="s">
-        <v>165</v>
-      </c>
-      <c r="B7" s="24"/>
-      <c r="D7" s="24" t="s">
+      <c r="A7" s="22" t="s">
+        <v>164</v>
+      </c>
+      <c r="B7" s="22"/>
+      <c r="D7" s="22" t="s">
         <v>127</v>
       </c>
-      <c r="E7" s="24"/>
-      <c r="G7" s="24" t="s">
+      <c r="E7" s="22"/>
+      <c r="G7" s="22" t="s">
         <v>128</v>
       </c>
-      <c r="H7" s="24"/>
-      <c r="L7" s="24" t="s">
+      <c r="H7" s="22"/>
+      <c r="L7" s="22" t="s">
         <v>142</v>
       </c>
-      <c r="M7" s="24"/>
+      <c r="M7" s="22"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
     </row>
     <row r="8" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A8" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B8" s="24"/>
-      <c r="C8" s="26" t="s">
+      <c r="A8" s="22" t="s">
+        <v>163</v>
+      </c>
+      <c r="B8" s="22"/>
+      <c r="C8" s="23" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="26"/>
-      <c r="E8" s="26" t="s">
+      <c r="D8" s="23"/>
+      <c r="E8" s="23" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="26"/>
-      <c r="G8" s="24" t="s">
+      <c r="F8" s="23"/>
+      <c r="G8" s="22" t="s">
         <v>132</v>
       </c>
-      <c r="H8" s="24"/>
-      <c r="K8" s="24" t="s">
+      <c r="H8" s="22"/>
+      <c r="K8" s="22" t="s">
         <v>143</v>
       </c>
-      <c r="L8" s="24"/>
-      <c r="M8" s="24" t="s">
+      <c r="L8" s="22"/>
+      <c r="M8" s="22" t="s">
         <v>144</v>
       </c>
-      <c r="N8" s="24"/>
+      <c r="N8" s="22"/>
       <c r="R8" s="20"/>
       <c r="S8" s="20"/>
       <c r="T8" s="20"/>
@@ -1404,18 +1487,18 @@
       <c r="Z8" s="20"/>
     </row>
     <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="24" t="s">
-        <v>163</v>
-      </c>
-      <c r="B9" s="24"/>
-      <c r="D9" s="24" t="s">
+      <c r="A9" s="22" t="s">
+        <v>162</v>
+      </c>
+      <c r="B9" s="22"/>
+      <c r="D9" s="22" t="s">
         <v>129</v>
       </c>
-      <c r="E9" s="24"/>
-      <c r="G9" s="24" t="s">
+      <c r="E9" s="22"/>
+      <c r="G9" s="22" t="s">
         <v>133</v>
       </c>
-      <c r="H9" s="24"/>
+      <c r="H9" s="22"/>
       <c r="N9" s="20"/>
       <c r="Q9" s="20"/>
       <c r="R9" s="20"/>
@@ -1430,10 +1513,10 @@
       <c r="AA9" s="20"/>
     </row>
     <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="22" t="s">
         <v>146</v>
       </c>
-      <c r="E10" s="24"/>
+      <c r="E10" s="22"/>
       <c r="N10" s="20"/>
       <c r="O10" s="20"/>
       <c r="P10" s="20"/>
@@ -1459,52 +1542,6 @@
     </row>
   </sheetData>
   <mergeCells count="63">
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D6:E6"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="C2:D2"/>
@@ -1521,7 +1558,53 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="L3:M3"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D6:E6"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J4:K4"/>
     <mergeCell ref="B4:C4"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -1537,7 +1620,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -14868,7 +14951,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Germany Focus Tree planning finished
</commit_message>
<xml_diff>
--- a/plans/Germany Focus Tree.xlsx
+++ b/plans/Germany Focus Tree.xlsx
@@ -21,6 +21,101 @@
     <author>Forfatter</author>
   </authors>
   <commentList>
+    <comment ref="AH1" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Six Year Plan mechanic: Every focus is available after a certain amount of time, depending on its row.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AD2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Requires both The Heer  and Six Year Plan</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AQ2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">Two decisions, </t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Focus on Production and Focus on Upgrades in terms of Air. One hastens production and the other improves air attack. Costs air experience.</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU2" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Unlocks the Rush Naval Production, which inceases naval building speed for navy experience</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="F3" authorId="0" shapeId="0">
       <text>
         <r>
@@ -69,6 +164,54 @@
         </r>
       </text>
     </comment>
+    <comment ref="AQ5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Air Exp generation</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AU5" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Naval Exp Generation</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="Z6" authorId="0" shapeId="0">
       <text>
         <r>
@@ -93,12 +236,60 @@
         </r>
       </text>
     </comment>
+    <comment ref="AP6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Interaction with the Heer and Airforce Specialty</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="AV6" authorId="0" shapeId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Forfatter:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Interaction with the Heer and Navy Specialty</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="236" uniqueCount="179">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="219">
   <si>
     <t>Illyria  Parties</t>
   </si>
@@ -571,9 +762,6 @@
     <t>Integrate the Austrians</t>
   </si>
   <si>
-    <t>Glorious German Army</t>
-  </si>
-  <si>
     <t>No Compromises</t>
   </si>
   <si>
@@ -589,9 +777,6 @@
     <t>Psychological Warfare</t>
   </si>
   <si>
-    <t>Address the People</t>
-  </si>
-  <si>
     <t>Goebbels' Administration</t>
   </si>
   <si>
@@ -625,9 +810,6 @@
     <t>Allow Foreigners to Join</t>
   </si>
   <si>
-    <t>Compulsive Service for the Occupied</t>
-  </si>
-  <si>
     <t>SS Cavalry Brigades</t>
   </si>
   <si>
@@ -635,6 +817,135 @@
   </si>
   <si>
     <t>SP Artillery</t>
+  </si>
+  <si>
+    <t>Aryans in Occupation Zones</t>
+  </si>
+  <si>
+    <t>Focus on Economy</t>
+  </si>
+  <si>
+    <t>Six Year Plan</t>
+  </si>
+  <si>
+    <t>Preparing the Fortifications</t>
+  </si>
+  <si>
+    <t>Fortify the Atlantic</t>
+  </si>
+  <si>
+    <t>Rush Fortification Production</t>
+  </si>
+  <si>
+    <t>Westwall Fortifications</t>
+  </si>
+  <si>
+    <t>Polish Border Fortifications</t>
+  </si>
+  <si>
+    <t>Lithuanian Border Fortifications</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Großraumwirtschaft </t>
+  </si>
+  <si>
+    <t>Start a Trade Circle</t>
+  </si>
+  <si>
+    <t>Autarky</t>
+  </si>
+  <si>
+    <t>Final Touches</t>
+  </si>
+  <si>
+    <t>Reichsautobahn</t>
+  </si>
+  <si>
+    <t>German War Economy</t>
+  </si>
+  <si>
+    <t>Coal Liquidization</t>
+  </si>
+  <si>
+    <t>Synthetic Materials</t>
+  </si>
+  <si>
+    <t>Science Effort</t>
+  </si>
+  <si>
+    <t>Wonder Weapons</t>
+  </si>
+  <si>
+    <t>Hermann-Goering Werke</t>
+  </si>
+  <si>
+    <t>KdF-Wagen</t>
+  </si>
+  <si>
+    <t>The Heer</t>
+  </si>
+  <si>
+    <t>The Luftwaffe</t>
+  </si>
+  <si>
+    <t>The Kriegsmarine</t>
+  </si>
+  <si>
+    <t>Airforce Specialty</t>
+  </si>
+  <si>
+    <t>Navy Specialty</t>
+  </si>
+  <si>
+    <t>Expand Dockyard Facilities</t>
+  </si>
+  <si>
+    <t>Interaction with the Heer</t>
+  </si>
+  <si>
+    <t>Marines</t>
+  </si>
+  <si>
+    <t>Paratroopers</t>
+  </si>
+  <si>
+    <t>Naval Bombers</t>
+  </si>
+  <si>
+    <t>Aircraft Carriers</t>
+  </si>
+  <si>
+    <t>Improve Model Designs</t>
+  </si>
+  <si>
+    <t>U-boats</t>
+  </si>
+  <si>
+    <t>Fighters</t>
+  </si>
+  <si>
+    <t>Experienced Airforce</t>
+  </si>
+  <si>
+    <t>Experienced Navy</t>
+  </si>
+  <si>
+    <t>Bombers</t>
+  </si>
+  <si>
+    <t>Airbase Construction</t>
+  </si>
+  <si>
+    <t>Air Doctrines</t>
+  </si>
+  <si>
+    <t>Naval Doctrines</t>
+  </si>
+  <si>
+    <t>Battleships</t>
+  </si>
+  <si>
+    <t>Naval Base Construction</t>
   </si>
 </sst>
 </file>
@@ -831,7 +1142,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
@@ -840,16 +1151,16 @@
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1192,10 +1503,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:AB12"/>
+  <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="R1" workbookViewId="0">
-      <selection activeCell="AF2" sqref="AF2"/>
+    <sheetView tabSelected="1" topLeftCell="AC2" workbookViewId="0">
+      <selection activeCell="AS4" sqref="AS4:AT4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -1203,23 +1514,35 @@
     <col min="1" max="16384" width="7.140625" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="28" t="s">
+      <c r="D1" s="23" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="28"/>
+      <c r="E1" s="23"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
       <c r="V1" s="22" t="s">
-        <v>157</v>
+        <v>197</v>
       </c>
       <c r="W1" s="22"/>
-    </row>
-    <row r="2" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH1" s="22" t="s">
+        <v>178</v>
+      </c>
+      <c r="AI1" s="22"/>
+      <c r="AP1" s="22" t="s">
+        <v>198</v>
+      </c>
+      <c r="AQ1" s="22"/>
+      <c r="AV1" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="AW1" s="22"/>
+    </row>
+    <row r="2" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
       <c r="C2" s="24" t="s">
@@ -1232,88 +1555,152 @@
       <c r="F2" s="24"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="29" t="s">
+      <c r="I2" s="28" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="29"/>
+      <c r="J2" s="28"/>
       <c r="R2" s="22" t="s">
         <v>147</v>
       </c>
       <c r="S2" s="22"/>
       <c r="V2" s="22" t="s">
-        <v>172</v>
+        <v>170</v>
       </c>
       <c r="W2" s="22"/>
       <c r="Z2" s="22" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="AA2" s="22"/>
-    </row>
-    <row r="3" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD2" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="AE2" s="22"/>
+      <c r="AG2" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="AH2" s="22"/>
+      <c r="AK2" s="22" t="s">
+        <v>187</v>
+      </c>
+      <c r="AL2" s="22"/>
+      <c r="AO2" s="24" t="s">
+        <v>210</v>
+      </c>
+      <c r="AP2" s="24"/>
+      <c r="AQ2" s="24" t="s">
+        <v>208</v>
+      </c>
+      <c r="AR2" s="24"/>
+      <c r="AS2" s="22" t="s">
+        <v>206</v>
+      </c>
+      <c r="AT2" s="22"/>
+      <c r="AU2" s="27" t="s">
+        <v>202</v>
+      </c>
+      <c r="AV2" s="27"/>
+      <c r="AW2" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="AX2" s="27"/>
+    </row>
+    <row r="3" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="23" t="s">
+      <c r="B3" s="27" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="23"/>
-      <c r="D3" s="23" t="s">
+      <c r="C3" s="27"/>
+      <c r="D3" s="27" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="23"/>
-      <c r="F3" s="23" t="s">
+      <c r="E3" s="27"/>
+      <c r="F3" s="27" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="23"/>
+      <c r="G3" s="27"/>
       <c r="H3" s="20"/>
-      <c r="L3" s="28" t="s">
+      <c r="L3" s="23" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="28"/>
-      <c r="Q3" s="27" t="s">
+      <c r="M3" s="23"/>
+      <c r="Q3" s="26" t="s">
         <v>148</v>
       </c>
-      <c r="R3" s="27"/>
-      <c r="S3" s="27" t="s">
+      <c r="R3" s="26"/>
+      <c r="S3" s="26" t="s">
         <v>154</v>
       </c>
-      <c r="T3" s="27"/>
+      <c r="T3" s="26"/>
       <c r="U3" s="25" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="V3" s="25"/>
       <c r="W3" s="25" t="s">
+        <v>172</v>
+      </c>
+      <c r="X3" s="25"/>
+      <c r="Y3" s="27" t="s">
         <v>174</v>
       </c>
-      <c r="X3" s="25"/>
-      <c r="Y3" s="23" t="s">
-        <v>177</v>
-      </c>
-      <c r="Z3" s="23"/>
-      <c r="AA3" s="23" t="s">
-        <v>167</v>
-      </c>
-      <c r="AB3" s="23"/>
-    </row>
-    <row r="4" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="28" t="s">
+      <c r="Z3" s="27"/>
+      <c r="AA3" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="AB3" s="27"/>
+      <c r="AC3" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="AD3" s="22"/>
+      <c r="AE3" s="22" t="s">
+        <v>183</v>
+      </c>
+      <c r="AF3" s="22"/>
+      <c r="AK3" s="22" t="s">
+        <v>191</v>
+      </c>
+      <c r="AL3" s="22"/>
+      <c r="AO3" s="27" t="s">
+        <v>214</v>
+      </c>
+      <c r="AP3" s="27"/>
+      <c r="AQ3" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="AR3" s="27"/>
+      <c r="AS3" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="AT3" s="22"/>
+      <c r="AU3" s="24" t="s">
+        <v>217</v>
+      </c>
+      <c r="AV3" s="24"/>
+      <c r="AW3" s="24" t="s">
+        <v>218</v>
+      </c>
+      <c r="AX3" s="24"/>
+    </row>
+    <row r="4" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B4" s="23" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="28"/>
+      <c r="C4" s="23"/>
       <c r="D4" s="22" t="s">
         <v>145</v>
       </c>
       <c r="E4" s="22"/>
-      <c r="F4" s="28" t="s">
+      <c r="F4" s="23" t="s">
         <v>156</v>
       </c>
-      <c r="G4" s="28"/>
+      <c r="G4" s="23"/>
       <c r="J4" s="22" t="s">
         <v>134</v>
       </c>
       <c r="K4" s="22"/>
-      <c r="N4" s="26" t="s">
+      <c r="N4" s="29" t="s">
         <v>138</v>
       </c>
-      <c r="O4" s="26"/>
+      <c r="O4" s="29"/>
       <c r="P4" s="21"/>
       <c r="Q4" s="22" t="s">
         <v>150</v>
@@ -1323,32 +1710,60 @@
         <v>153</v>
       </c>
       <c r="T4" s="22"/>
-      <c r="U4" s="23" t="s">
+      <c r="U4" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="V4" s="27"/>
+      <c r="W4" s="27" t="s">
         <v>173</v>
       </c>
-      <c r="V4" s="23"/>
-      <c r="W4" s="23" t="s">
-        <v>176</v>
-      </c>
-      <c r="X4" s="23"/>
+      <c r="X4" s="27"/>
       <c r="Y4" s="24" t="s">
-        <v>178</v>
+        <v>175</v>
       </c>
       <c r="Z4" s="24"/>
       <c r="AA4" s="24" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="AB4" s="24"/>
-    </row>
-    <row r="5" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="23" t="s">
+      <c r="AG4" s="22" t="s">
+        <v>186</v>
+      </c>
+      <c r="AH4" s="22"/>
+      <c r="AI4" s="22" t="s">
+        <v>189</v>
+      </c>
+      <c r="AJ4" s="22"/>
+      <c r="AK4" s="22" t="s">
+        <v>192</v>
+      </c>
+      <c r="AL4" s="22"/>
+      <c r="AM4" s="22" t="s">
+        <v>195</v>
+      </c>
+      <c r="AN4" s="22"/>
+      <c r="AP4" s="22" t="s">
+        <v>200</v>
+      </c>
+      <c r="AQ4" s="22"/>
+      <c r="AS4" s="22" t="s">
+        <v>203</v>
+      </c>
+      <c r="AT4" s="22"/>
+      <c r="AV4" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="AW4" s="22"/>
+    </row>
+    <row r="5" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="23"/>
-      <c r="C5" s="23" t="s">
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="23"/>
+      <c r="D5" s="27"/>
       <c r="E5" s="24" t="s">
         <v>152</v>
       </c>
@@ -1361,55 +1776,83 @@
         <v>135</v>
       </c>
       <c r="K5" s="22"/>
-      <c r="N5" s="26" t="s">
+      <c r="N5" s="29" t="s">
         <v>139</v>
       </c>
-      <c r="O5" s="26"/>
+      <c r="O5" s="29"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="22" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="R5" s="22"/>
       <c r="S5" s="22" t="s">
-        <v>171</v>
+        <v>169</v>
       </c>
       <c r="T5" s="22"/>
       <c r="U5" s="24" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="V5" s="24"/>
       <c r="W5" s="24" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="X5" s="24"/>
-      <c r="Y5" s="23" t="s">
-        <v>166</v>
-      </c>
-      <c r="Z5" s="23"/>
-      <c r="AA5" s="23" t="s">
-        <v>169</v>
-      </c>
-      <c r="AB5" s="23"/>
-    </row>
-    <row r="6" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="Y5" s="27" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z5" s="27"/>
+      <c r="AA5" s="27" t="s">
+        <v>167</v>
+      </c>
+      <c r="AB5" s="27"/>
+      <c r="AC5" s="22" t="s">
+        <v>180</v>
+      </c>
+      <c r="AD5" s="22"/>
+      <c r="AE5" s="22" t="s">
+        <v>184</v>
+      </c>
+      <c r="AF5" s="22"/>
+      <c r="AK5" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="AL5" s="22"/>
+      <c r="AO5" s="24" t="s">
+        <v>215</v>
+      </c>
+      <c r="AP5" s="24"/>
+      <c r="AQ5" s="24" t="s">
+        <v>211</v>
+      </c>
+      <c r="AR5" s="24"/>
+      <c r="AU5" s="27" t="s">
+        <v>212</v>
+      </c>
+      <c r="AV5" s="27"/>
+      <c r="AW5" s="27" t="s">
+        <v>216</v>
+      </c>
+      <c r="AX5" s="27"/>
+    </row>
+    <row r="6" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="29" t="s">
+      <c r="D6" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="29"/>
+      <c r="E6" s="28"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="27" t="s">
+      <c r="I6" s="26" t="s">
         <v>136</v>
       </c>
-      <c r="J6" s="27"/>
-      <c r="K6" s="27" t="s">
+      <c r="J6" s="26"/>
+      <c r="K6" s="26" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="27"/>
+      <c r="L6" s="26"/>
       <c r="M6" s="25" t="s">
         <v>140</v>
       </c>
@@ -1423,17 +1866,41 @@
       </c>
       <c r="S6" s="22"/>
       <c r="V6" s="22" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="W6" s="22"/>
       <c r="Z6" s="22" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="AA6" s="22"/>
-    </row>
-    <row r="7" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AD6" s="22" t="s">
+        <v>181</v>
+      </c>
+      <c r="AE6" s="22"/>
+      <c r="AI6" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="AJ6" s="22"/>
+      <c r="AK6" s="22" t="s">
+        <v>194</v>
+      </c>
+      <c r="AL6" s="22"/>
+      <c r="AM6" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="AN6" s="22"/>
+      <c r="AP6" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="AQ6" s="22"/>
+      <c r="AV6" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="AW6" s="22"/>
+    </row>
+    <row r="7" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="22" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B7" s="22"/>
       <c r="D7" s="22" t="s">
@@ -1450,20 +1917,24 @@
       <c r="M7" s="22"/>
       <c r="X7" s="20"/>
       <c r="Y7" s="20"/>
-    </row>
-    <row r="8" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="AH7" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="AI7" s="22"/>
+    </row>
+    <row r="8" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="22" t="s">
-        <v>163</v>
+        <v>133</v>
       </c>
       <c r="B8" s="22"/>
-      <c r="C8" s="23" t="s">
+      <c r="C8" s="27" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="23"/>
-      <c r="E8" s="23" t="s">
+      <c r="D8" s="27"/>
+      <c r="E8" s="27" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="23"/>
+      <c r="F8" s="27"/>
       <c r="G8" s="22" t="s">
         <v>132</v>
       </c>
@@ -1486,9 +1957,9 @@
       <c r="Y8" s="20"/>
       <c r="Z8" s="20"/>
     </row>
-    <row r="9" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B9" s="22"/>
       <c r="D9" s="22" t="s">
@@ -1496,7 +1967,7 @@
       </c>
       <c r="E9" s="22"/>
       <c r="G9" s="22" t="s">
-        <v>133</v>
+        <v>177</v>
       </c>
       <c r="H9" s="22"/>
       <c r="N9" s="20"/>
@@ -1512,7 +1983,7 @@
       <c r="Z9" s="20"/>
       <c r="AA9" s="20"/>
     </row>
-    <row r="10" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="D10" s="22" t="s">
         <v>146</v>
       </c>
@@ -1524,7 +1995,7 @@
       <c r="Z10" s="20"/>
       <c r="AA10" s="20"/>
     </row>
-    <row r="11" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N11" s="20"/>
       <c r="O11" s="20"/>
       <c r="P11" s="20"/>
@@ -1532,7 +2003,7 @@
       <c r="Z11" s="20"/>
       <c r="AA11" s="20"/>
     </row>
-    <row r="12" spans="1:28" ht="75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="N12" s="20"/>
       <c r="O12" s="20"/>
       <c r="P12" s="20"/>
@@ -1541,7 +2012,94 @@
       <c r="AA12" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="63">
+  <mergeCells count="103">
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AV6:AW6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AV4:AW4"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AO5:AP5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="A5:B5"/>
+    <mergeCell ref="G5:H5"/>
+    <mergeCell ref="E5:F5"/>
+    <mergeCell ref="C5:D5"/>
+    <mergeCell ref="J4:K4"/>
+    <mergeCell ref="B4:C4"/>
+    <mergeCell ref="D10:E10"/>
+    <mergeCell ref="O6:P6"/>
+    <mergeCell ref="K8:L8"/>
+    <mergeCell ref="M8:N8"/>
+    <mergeCell ref="D4:E4"/>
+    <mergeCell ref="L7:M7"/>
+    <mergeCell ref="N4:O4"/>
+    <mergeCell ref="J5:K5"/>
+    <mergeCell ref="I6:J6"/>
+    <mergeCell ref="K6:L6"/>
+    <mergeCell ref="N5:O5"/>
+    <mergeCell ref="F4:G4"/>
+    <mergeCell ref="D6:E6"/>
     <mergeCell ref="Q5:R5"/>
     <mergeCell ref="D1:E1"/>
     <mergeCell ref="C2:D2"/>
@@ -1558,53 +2116,6 @@
     <mergeCell ref="F3:G3"/>
     <mergeCell ref="I2:J2"/>
     <mergeCell ref="L3:M3"/>
-    <mergeCell ref="D10:E10"/>
-    <mergeCell ref="O6:P6"/>
-    <mergeCell ref="K8:L8"/>
-    <mergeCell ref="M8:N8"/>
-    <mergeCell ref="D4:E4"/>
-    <mergeCell ref="L7:M7"/>
-    <mergeCell ref="N4:O4"/>
-    <mergeCell ref="J5:K5"/>
-    <mergeCell ref="I6:J6"/>
-    <mergeCell ref="K6:L6"/>
-    <mergeCell ref="N5:O5"/>
-    <mergeCell ref="F4:G4"/>
-    <mergeCell ref="D6:E6"/>
-    <mergeCell ref="A5:B5"/>
-    <mergeCell ref="G5:H5"/>
-    <mergeCell ref="E5:F5"/>
-    <mergeCell ref="C5:D5"/>
-    <mergeCell ref="J4:K4"/>
-    <mergeCell ref="B4:C4"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="D9:E9"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
german focus tree edits
</commit_message>
<xml_diff>
--- a/plans/Germany Focus Tree.xlsx
+++ b/plans/Germany Focus Tree.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="18431"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7530"/>
@@ -18,10 +18,10 @@
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
 <comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <authors>
-    <author>Forfatter</author>
+    <author>Author</author>
   </authors>
   <commentList>
-    <comment ref="AH1" authorId="0" shapeId="0">
+    <comment ref="AH1" authorId="0">
       <text>
         <r>
           <rPr>
@@ -31,7 +31,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -45,7 +45,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AD2" authorId="0" shapeId="0">
+    <comment ref="AD2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -55,7 +55,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -69,7 +69,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ2" authorId="0" shapeId="0">
+    <comment ref="AQ2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -92,7 +92,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU2" authorId="0" shapeId="0">
+    <comment ref="AU2" authorId="0">
       <text>
         <r>
           <rPr>
@@ -102,7 +102,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -116,7 +116,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="F3" authorId="0" shapeId="0">
+    <comment ref="F3" authorId="0">
       <text>
         <r>
           <rPr>
@@ -126,7 +126,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -140,7 +140,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="D4" authorId="0" shapeId="0">
+    <comment ref="D4" authorId="0">
       <text>
         <r>
           <rPr>
@@ -150,7 +150,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -164,7 +164,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AQ5" authorId="0" shapeId="0">
+    <comment ref="AQ5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -174,7 +174,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -188,7 +188,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AU5" authorId="0" shapeId="0">
+    <comment ref="AU5" authorId="0">
       <text>
         <r>
           <rPr>
@@ -198,7 +198,7 @@
             <rFont val="Tahoma"/>
             <family val="2"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -212,7 +212,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="Z6" authorId="0" shapeId="0">
+    <comment ref="Z6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -222,7 +222,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -236,7 +236,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AP6" authorId="0" shapeId="0">
+    <comment ref="AP6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -246,7 +246,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -260,7 +260,7 @@
         </r>
       </text>
     </comment>
-    <comment ref="AV6" authorId="0" shapeId="0">
+    <comment ref="AV6" authorId="0">
       <text>
         <r>
           <rPr>
@@ -270,7 +270,7 @@
             <rFont val="Tahoma"/>
             <charset val="1"/>
           </rPr>
-          <t>Forfatter:</t>
+          <t>Author:</t>
         </r>
         <r>
           <rPr>
@@ -284,12 +284,156 @@
         </r>
       </text>
     </comment>
+    <comment ref="X8" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Lowers world tension, liked by all countries of opposing ideology</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X9" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Germanic Migration idea (monthly pop), and adds a significant amount of manpower</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="P10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Gives Norway to Sweden and puppets them, if they agree</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="R10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Core any european state over a huge period of time</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="T10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Partitions Belgium with Petain's France</t>
+        </r>
+      </text>
+    </comment>
+    <comment ref="X10" authorId="0">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t>Author:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <charset val="1"/>
+          </rPr>
+          <t xml:space="preserve">
+Unlocks Germanization decisions</t>
+        </r>
+      </text>
+    </comment>
   </commentList>
 </comments>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="276" uniqueCount="219">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="292" uniqueCount="235">
   <si>
     <t>Illyria  Parties</t>
   </si>
@@ -946,12 +1090,60 @@
   </si>
   <si>
     <t>Naval Base Construction</t>
+  </si>
+  <si>
+    <t>Hypergermanism</t>
+  </si>
+  <si>
+    <t>Stronghold of the Germanic</t>
+  </si>
+  <si>
+    <t>Invite Germanic Immigrants</t>
+  </si>
+  <si>
+    <t>Ancient Lineage</t>
+  </si>
+  <si>
+    <t>Northern Germans</t>
+  </si>
+  <si>
+    <t>The Dutch</t>
+  </si>
+  <si>
+    <t>Annex Netherlands</t>
+  </si>
+  <si>
+    <t>Partition Belgium</t>
+  </si>
+  <si>
+    <t>Annex Flanders</t>
+  </si>
+  <si>
+    <t>Occupation of Sweden</t>
+  </si>
+  <si>
+    <t>From Atlantic to the Urals</t>
+  </si>
+  <si>
+    <t>Norway for Allegiance</t>
+  </si>
+  <si>
+    <t>Occupation of Denmark</t>
+  </si>
+  <si>
+    <t>Occupation of Norway</t>
+  </si>
+  <si>
+    <t>Ease Expansionism</t>
+  </si>
+  <si>
+    <t>Germanize Minorities</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="16" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -1094,10 +1286,19 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -1108,7 +1309,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="30">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -1142,30 +1343,33 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="6" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
-    <cellStyle name="Hyperkobling" xfId="2" builtinId="8"/>
+    <cellStyle name="Hyperlink" xfId="2" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1"/>
   </cellStyles>
@@ -1183,7 +1387,7 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office-tema">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -1225,7 +1429,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1258,26 +1462,9 @@
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -1310,23 +1497,6 @@
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
         <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -1505,11 +1675,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:AX12"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="AC2" workbookViewId="0">
-      <selection activeCell="AS4" sqref="AS4:AT4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="U9" sqref="U9:V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="7.140625" defaultRowHeight="75" customHeight="1" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="16384" width="7.140625" style="1"/>
   </cols>
@@ -1518,10 +1688,10 @@
       <c r="A1" s="20"/>
       <c r="B1" s="20"/>
       <c r="C1" s="20"/>
-      <c r="D1" s="23" t="s">
+      <c r="D1" s="26" t="s">
         <v>116</v>
       </c>
-      <c r="E1" s="23"/>
+      <c r="E1" s="26"/>
       <c r="F1" s="20"/>
       <c r="G1" s="20"/>
       <c r="H1" s="20"/>
@@ -1545,20 +1715,20 @@
     <row r="2" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="20"/>
       <c r="B2" s="20"/>
-      <c r="C2" s="24" t="s">
+      <c r="C2" s="23" t="s">
         <v>117</v>
       </c>
-      <c r="D2" s="24"/>
-      <c r="E2" s="24" t="s">
+      <c r="D2" s="23"/>
+      <c r="E2" s="23" t="s">
         <v>155</v>
       </c>
-      <c r="F2" s="24"/>
+      <c r="F2" s="23"/>
       <c r="G2" s="20"/>
       <c r="H2" s="20"/>
-      <c r="I2" s="28" t="s">
+      <c r="I2" s="29" t="s">
         <v>120</v>
       </c>
-      <c r="J2" s="28"/>
+      <c r="J2" s="29"/>
       <c r="R2" s="22" t="s">
         <v>147</v>
       </c>
@@ -1583,54 +1753,54 @@
         <v>187</v>
       </c>
       <c r="AL2" s="22"/>
-      <c r="AO2" s="24" t="s">
+      <c r="AO2" s="23" t="s">
         <v>210</v>
       </c>
-      <c r="AP2" s="24"/>
-      <c r="AQ2" s="24" t="s">
+      <c r="AP2" s="23"/>
+      <c r="AQ2" s="23" t="s">
         <v>208</v>
       </c>
-      <c r="AR2" s="24"/>
+      <c r="AR2" s="23"/>
       <c r="AS2" s="22" t="s">
         <v>206</v>
       </c>
       <c r="AT2" s="22"/>
-      <c r="AU2" s="27" t="s">
+      <c r="AU2" s="24" t="s">
         <v>202</v>
       </c>
-      <c r="AV2" s="27"/>
-      <c r="AW2" s="27" t="s">
+      <c r="AV2" s="24"/>
+      <c r="AW2" s="24" t="s">
         <v>209</v>
       </c>
-      <c r="AX2" s="27"/>
+      <c r="AX2" s="24"/>
     </row>
     <row r="3" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="20"/>
-      <c r="B3" s="27" t="s">
+      <c r="B3" s="24" t="s">
         <v>119</v>
       </c>
-      <c r="C3" s="27"/>
-      <c r="D3" s="27" t="s">
+      <c r="C3" s="24"/>
+      <c r="D3" s="24" t="s">
         <v>118</v>
       </c>
-      <c r="E3" s="27"/>
-      <c r="F3" s="27" t="s">
+      <c r="E3" s="24"/>
+      <c r="F3" s="24" t="s">
         <v>121</v>
       </c>
-      <c r="G3" s="27"/>
+      <c r="G3" s="24"/>
       <c r="H3" s="20"/>
-      <c r="L3" s="23" t="s">
+      <c r="L3" s="26" t="s">
         <v>122</v>
       </c>
-      <c r="M3" s="23"/>
-      <c r="Q3" s="26" t="s">
+      <c r="M3" s="26"/>
+      <c r="Q3" s="28" t="s">
         <v>148</v>
       </c>
-      <c r="R3" s="26"/>
-      <c r="S3" s="26" t="s">
+      <c r="R3" s="28"/>
+      <c r="S3" s="28" t="s">
         <v>154</v>
       </c>
-      <c r="T3" s="26"/>
+      <c r="T3" s="28"/>
       <c r="U3" s="25" t="s">
         <v>157</v>
       </c>
@@ -1639,14 +1809,14 @@
         <v>172</v>
       </c>
       <c r="X3" s="25"/>
-      <c r="Y3" s="27" t="s">
+      <c r="Y3" s="24" t="s">
         <v>174</v>
       </c>
-      <c r="Z3" s="27"/>
-      <c r="AA3" s="27" t="s">
+      <c r="Z3" s="24"/>
+      <c r="AA3" s="24" t="s">
         <v>165</v>
       </c>
-      <c r="AB3" s="27"/>
+      <c r="AB3" s="24"/>
       <c r="AC3" s="22" t="s">
         <v>182</v>
       </c>
@@ -1659,48 +1829,48 @@
         <v>191</v>
       </c>
       <c r="AL3" s="22"/>
-      <c r="AO3" s="27" t="s">
+      <c r="AO3" s="24" t="s">
         <v>214</v>
       </c>
-      <c r="AP3" s="27"/>
-      <c r="AQ3" s="27" t="s">
+      <c r="AP3" s="24"/>
+      <c r="AQ3" s="24" t="s">
         <v>213</v>
       </c>
-      <c r="AR3" s="27"/>
+      <c r="AR3" s="24"/>
       <c r="AS3" s="22" t="s">
         <v>207</v>
       </c>
       <c r="AT3" s="22"/>
-      <c r="AU3" s="24" t="s">
+      <c r="AU3" s="23" t="s">
         <v>217</v>
       </c>
-      <c r="AV3" s="24"/>
-      <c r="AW3" s="24" t="s">
+      <c r="AV3" s="23"/>
+      <c r="AW3" s="23" t="s">
         <v>218</v>
       </c>
-      <c r="AX3" s="24"/>
+      <c r="AX3" s="23"/>
     </row>
     <row r="4" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B4" s="23" t="s">
+      <c r="B4" s="26" t="s">
         <v>125</v>
       </c>
-      <c r="C4" s="23"/>
+      <c r="C4" s="26"/>
       <c r="D4" s="22" t="s">
         <v>145</v>
       </c>
       <c r="E4" s="22"/>
-      <c r="F4" s="23" t="s">
+      <c r="F4" s="26" t="s">
         <v>156</v>
       </c>
-      <c r="G4" s="23"/>
+      <c r="G4" s="26"/>
       <c r="J4" s="22" t="s">
         <v>134</v>
       </c>
       <c r="K4" s="22"/>
-      <c r="N4" s="29" t="s">
+      <c r="N4" s="27" t="s">
         <v>138</v>
       </c>
-      <c r="O4" s="29"/>
+      <c r="O4" s="27"/>
       <c r="P4" s="21"/>
       <c r="Q4" s="22" t="s">
         <v>150</v>
@@ -1710,22 +1880,22 @@
         <v>153</v>
       </c>
       <c r="T4" s="22"/>
-      <c r="U4" s="27" t="s">
+      <c r="U4" s="24" t="s">
         <v>171</v>
       </c>
-      <c r="V4" s="27"/>
-      <c r="W4" s="27" t="s">
+      <c r="V4" s="24"/>
+      <c r="W4" s="24" t="s">
         <v>173</v>
       </c>
-      <c r="X4" s="27"/>
-      <c r="Y4" s="24" t="s">
+      <c r="X4" s="24"/>
+      <c r="Y4" s="23" t="s">
         <v>175</v>
       </c>
-      <c r="Z4" s="24"/>
-      <c r="AA4" s="24" t="s">
+      <c r="Z4" s="23"/>
+      <c r="AA4" s="23" t="s">
         <v>166</v>
       </c>
-      <c r="AB4" s="24"/>
+      <c r="AB4" s="23"/>
       <c r="AG4" s="22" t="s">
         <v>186</v>
       </c>
@@ -1756,30 +1926,30 @@
       <c r="AW4" s="22"/>
     </row>
     <row r="5" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="27" t="s">
+      <c r="A5" s="24" t="s">
         <v>124</v>
       </c>
-      <c r="B5" s="27"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="24"/>
+      <c r="C5" s="24" t="s">
         <v>126</v>
       </c>
-      <c r="D5" s="27"/>
-      <c r="E5" s="24" t="s">
+      <c r="D5" s="24"/>
+      <c r="E5" s="23" t="s">
         <v>152</v>
       </c>
-      <c r="F5" s="24"/>
-      <c r="G5" s="24" t="s">
+      <c r="F5" s="23"/>
+      <c r="G5" s="23" t="s">
         <v>151</v>
       </c>
-      <c r="H5" s="24"/>
+      <c r="H5" s="23"/>
       <c r="J5" s="22" t="s">
         <v>135</v>
       </c>
       <c r="K5" s="22"/>
-      <c r="N5" s="29" t="s">
+      <c r="N5" s="27" t="s">
         <v>139</v>
       </c>
-      <c r="O5" s="29"/>
+      <c r="O5" s="27"/>
       <c r="P5" s="21"/>
       <c r="Q5" s="22" t="s">
         <v>168</v>
@@ -1789,22 +1959,22 @@
         <v>169</v>
       </c>
       <c r="T5" s="22"/>
-      <c r="U5" s="24" t="s">
+      <c r="U5" s="23" t="s">
         <v>163</v>
       </c>
-      <c r="V5" s="24"/>
-      <c r="W5" s="24" t="s">
+      <c r="V5" s="23"/>
+      <c r="W5" s="23" t="s">
         <v>158</v>
       </c>
-      <c r="X5" s="24"/>
-      <c r="Y5" s="27" t="s">
+      <c r="X5" s="23"/>
+      <c r="Y5" s="24" t="s">
         <v>164</v>
       </c>
-      <c r="Z5" s="27"/>
-      <c r="AA5" s="27" t="s">
+      <c r="Z5" s="24"/>
+      <c r="AA5" s="24" t="s">
         <v>167</v>
       </c>
-      <c r="AB5" s="27"/>
+      <c r="AB5" s="24"/>
       <c r="AC5" s="22" t="s">
         <v>180</v>
       </c>
@@ -1817,42 +1987,42 @@
         <v>193</v>
       </c>
       <c r="AL5" s="22"/>
-      <c r="AO5" s="24" t="s">
+      <c r="AO5" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="AP5" s="24"/>
-      <c r="AQ5" s="24" t="s">
+      <c r="AP5" s="23"/>
+      <c r="AQ5" s="23" t="s">
         <v>211</v>
       </c>
-      <c r="AR5" s="24"/>
-      <c r="AU5" s="27" t="s">
+      <c r="AR5" s="23"/>
+      <c r="AU5" s="24" t="s">
         <v>212</v>
       </c>
-      <c r="AV5" s="27"/>
-      <c r="AW5" s="27" t="s">
+      <c r="AV5" s="24"/>
+      <c r="AW5" s="24" t="s">
         <v>216</v>
       </c>
-      <c r="AX5" s="27"/>
+      <c r="AX5" s="24"/>
     </row>
     <row r="6" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="20"/>
       <c r="B6" s="20"/>
       <c r="C6" s="20"/>
-      <c r="D6" s="28" t="s">
+      <c r="D6" s="29" t="s">
         <v>123</v>
       </c>
-      <c r="E6" s="28"/>
+      <c r="E6" s="29"/>
       <c r="F6" s="20"/>
       <c r="G6" s="20"/>
       <c r="H6" s="20"/>
-      <c r="I6" s="26" t="s">
+      <c r="I6" s="28" t="s">
         <v>136</v>
       </c>
-      <c r="J6" s="26"/>
-      <c r="K6" s="26" t="s">
+      <c r="J6" s="28"/>
+      <c r="K6" s="28" t="s">
         <v>137</v>
       </c>
-      <c r="L6" s="26"/>
+      <c r="L6" s="28"/>
       <c r="M6" s="25" t="s">
         <v>140</v>
       </c>
@@ -1915,8 +2085,14 @@
         <v>142</v>
       </c>
       <c r="M7" s="22"/>
-      <c r="X7" s="20"/>
-      <c r="Y7" s="20"/>
+      <c r="R7" s="28" t="s">
+        <v>219</v>
+      </c>
+      <c r="S7" s="28"/>
+      <c r="X7" s="28" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y7" s="28"/>
       <c r="AH7" s="22" t="s">
         <v>188</v>
       </c>
@@ -1927,14 +2103,14 @@
         <v>133</v>
       </c>
       <c r="B8" s="22"/>
-      <c r="C8" s="27" t="s">
+      <c r="C8" s="24" t="s">
         <v>130</v>
       </c>
-      <c r="D8" s="27"/>
-      <c r="E8" s="27" t="s">
+      <c r="D8" s="24"/>
+      <c r="E8" s="24" t="s">
         <v>131</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="24"/>
       <c r="G8" s="22" t="s">
         <v>132</v>
       </c>
@@ -1943,19 +2119,27 @@
         <v>143</v>
       </c>
       <c r="L8" s="22"/>
-      <c r="M8" s="22" t="s">
+      <c r="M8" s="27" t="s">
         <v>144</v>
       </c>
-      <c r="N8" s="22"/>
-      <c r="R8" s="20"/>
-      <c r="S8" s="20"/>
-      <c r="T8" s="20"/>
-      <c r="U8" s="20"/>
-      <c r="V8" s="20"/>
+      <c r="N8" s="30"/>
+      <c r="P8" s="22" t="s">
+        <v>223</v>
+      </c>
+      <c r="Q8" s="22"/>
+      <c r="R8" s="26" t="s">
+        <v>222</v>
+      </c>
+      <c r="S8" s="26"/>
+      <c r="U8" s="22" t="s">
+        <v>224</v>
+      </c>
+      <c r="V8" s="22"/>
       <c r="W8" s="20"/>
-      <c r="X8" s="20"/>
-      <c r="Y8" s="20"/>
-      <c r="Z8" s="20"/>
+      <c r="X8" s="26" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y8" s="26"/>
     </row>
     <row r="9" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="22" t="s">
@@ -1971,16 +2155,23 @@
       </c>
       <c r="H9" s="22"/>
       <c r="N9" s="20"/>
-      <c r="Q9" s="20"/>
-      <c r="R9" s="20"/>
-      <c r="S9" s="20"/>
-      <c r="T9" s="20"/>
-      <c r="U9" s="20"/>
-      <c r="V9" s="20"/>
+      <c r="O9" s="26" t="s">
+        <v>232</v>
+      </c>
+      <c r="P9" s="26"/>
+      <c r="Q9" s="22" t="s">
+        <v>231</v>
+      </c>
+      <c r="R9" s="22"/>
+      <c r="U9" s="22" t="s">
+        <v>225</v>
+      </c>
+      <c r="V9" s="22"/>
       <c r="W9" s="20"/>
-      <c r="X9" s="20"/>
-      <c r="Y9" s="20"/>
-      <c r="Z9" s="20"/>
+      <c r="X9" s="26" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y9" s="26"/>
       <c r="AA9" s="20"/>
     </row>
     <row r="10" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1988,11 +2179,30 @@
         <v>146</v>
       </c>
       <c r="E10" s="22"/>
-      <c r="N10" s="20"/>
-      <c r="O10" s="20"/>
-      <c r="P10" s="20"/>
-      <c r="Y10" s="20"/>
-      <c r="Z10" s="20"/>
+      <c r="N10" s="28" t="s">
+        <v>228</v>
+      </c>
+      <c r="O10" s="28"/>
+      <c r="P10" s="28" t="s">
+        <v>230</v>
+      </c>
+      <c r="Q10" s="28"/>
+      <c r="R10" s="22" t="s">
+        <v>229</v>
+      </c>
+      <c r="S10" s="22"/>
+      <c r="T10" s="25" t="s">
+        <v>226</v>
+      </c>
+      <c r="U10" s="25"/>
+      <c r="V10" s="25" t="s">
+        <v>227</v>
+      </c>
+      <c r="W10" s="25"/>
+      <c r="X10" s="26" t="s">
+        <v>234</v>
+      </c>
+      <c r="Y10" s="26"/>
       <c r="AA10" s="20"/>
     </row>
     <row r="11" spans="1:50" ht="75" customHeight="1" x14ac:dyDescent="0.25">
@@ -2012,75 +2222,38 @@
       <c r="AA12" s="20"/>
     </row>
   </sheetData>
-  <mergeCells count="103">
-    <mergeCell ref="AS2:AT2"/>
-    <mergeCell ref="AS3:AT3"/>
-    <mergeCell ref="AQ5:AR5"/>
-    <mergeCell ref="AU5:AV5"/>
-    <mergeCell ref="AW5:AX5"/>
-    <mergeCell ref="AS4:AT4"/>
-    <mergeCell ref="AV6:AW6"/>
-    <mergeCell ref="AP6:AQ6"/>
-    <mergeCell ref="AH7:AI7"/>
-    <mergeCell ref="AK4:AL4"/>
-    <mergeCell ref="AK6:AL6"/>
-    <mergeCell ref="AP1:AQ1"/>
-    <mergeCell ref="AV1:AW1"/>
-    <mergeCell ref="AP4:AQ4"/>
-    <mergeCell ref="AV4:AW4"/>
-    <mergeCell ref="AQ2:AR2"/>
-    <mergeCell ref="AO2:AP2"/>
-    <mergeCell ref="AO3:AP3"/>
-    <mergeCell ref="AQ3:AR3"/>
-    <mergeCell ref="AU2:AV2"/>
-    <mergeCell ref="AW2:AX2"/>
-    <mergeCell ref="AU3:AV3"/>
-    <mergeCell ref="AW3:AX3"/>
-    <mergeCell ref="AO5:AP5"/>
-    <mergeCell ref="AD6:AE6"/>
-    <mergeCell ref="AG2:AH2"/>
-    <mergeCell ref="AG4:AH4"/>
-    <mergeCell ref="AK2:AL2"/>
-    <mergeCell ref="AI4:AJ4"/>
-    <mergeCell ref="AK3:AL3"/>
-    <mergeCell ref="AM4:AN4"/>
-    <mergeCell ref="AI6:AJ6"/>
-    <mergeCell ref="AM6:AN6"/>
-    <mergeCell ref="AK5:AL5"/>
-    <mergeCell ref="AH1:AI1"/>
-    <mergeCell ref="AD2:AE2"/>
-    <mergeCell ref="AC3:AD3"/>
-    <mergeCell ref="AE3:AF3"/>
-    <mergeCell ref="AE5:AF5"/>
-    <mergeCell ref="AC5:AD5"/>
-    <mergeCell ref="S5:T5"/>
-    <mergeCell ref="U4:V4"/>
-    <mergeCell ref="W4:X4"/>
-    <mergeCell ref="U5:V5"/>
-    <mergeCell ref="W5:X5"/>
-    <mergeCell ref="V6:W6"/>
-    <mergeCell ref="Z6:AA6"/>
-    <mergeCell ref="Y4:Z4"/>
-    <mergeCell ref="AA4:AB4"/>
-    <mergeCell ref="Y5:Z5"/>
-    <mergeCell ref="AA5:AB5"/>
-    <mergeCell ref="V1:W1"/>
-    <mergeCell ref="V2:W2"/>
-    <mergeCell ref="U3:V3"/>
-    <mergeCell ref="W3:X3"/>
-    <mergeCell ref="Z2:AA2"/>
-    <mergeCell ref="Y3:Z3"/>
-    <mergeCell ref="AA3:AB3"/>
-    <mergeCell ref="A7:B7"/>
-    <mergeCell ref="G7:H7"/>
-    <mergeCell ref="D7:E7"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="C8:D8"/>
-    <mergeCell ref="E8:F8"/>
-    <mergeCell ref="G8:H8"/>
-    <mergeCell ref="G9:H9"/>
-    <mergeCell ref="D9:E9"/>
+  <mergeCells count="119">
+    <mergeCell ref="T10:U10"/>
+    <mergeCell ref="V10:W10"/>
+    <mergeCell ref="R10:S10"/>
+    <mergeCell ref="P10:Q10"/>
+    <mergeCell ref="N10:O10"/>
+    <mergeCell ref="X10:Y10"/>
+    <mergeCell ref="X7:Y7"/>
+    <mergeCell ref="U8:V8"/>
+    <mergeCell ref="R8:S8"/>
+    <mergeCell ref="P8:Q8"/>
+    <mergeCell ref="X8:Y8"/>
+    <mergeCell ref="X9:Y9"/>
+    <mergeCell ref="O9:P9"/>
+    <mergeCell ref="Q9:R9"/>
+    <mergeCell ref="U9:V9"/>
+    <mergeCell ref="Q5:R5"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="C2:D2"/>
+    <mergeCell ref="E2:F2"/>
+    <mergeCell ref="M6:N6"/>
+    <mergeCell ref="R2:S2"/>
+    <mergeCell ref="Q3:R3"/>
+    <mergeCell ref="S3:T3"/>
+    <mergeCell ref="Q4:R4"/>
+    <mergeCell ref="S4:T4"/>
+    <mergeCell ref="R6:S6"/>
+    <mergeCell ref="D3:E3"/>
+    <mergeCell ref="B3:C3"/>
+    <mergeCell ref="F3:G3"/>
+    <mergeCell ref="I2:J2"/>
+    <mergeCell ref="L3:M3"/>
     <mergeCell ref="A5:B5"/>
     <mergeCell ref="G5:H5"/>
     <mergeCell ref="E5:F5"/>
@@ -2100,22 +2273,75 @@
     <mergeCell ref="N5:O5"/>
     <mergeCell ref="F4:G4"/>
     <mergeCell ref="D6:E6"/>
-    <mergeCell ref="Q5:R5"/>
-    <mergeCell ref="D1:E1"/>
-    <mergeCell ref="C2:D2"/>
-    <mergeCell ref="E2:F2"/>
-    <mergeCell ref="M6:N6"/>
-    <mergeCell ref="R2:S2"/>
-    <mergeCell ref="Q3:R3"/>
-    <mergeCell ref="S3:T3"/>
-    <mergeCell ref="Q4:R4"/>
-    <mergeCell ref="S4:T4"/>
-    <mergeCell ref="R6:S6"/>
-    <mergeCell ref="D3:E3"/>
-    <mergeCell ref="B3:C3"/>
-    <mergeCell ref="F3:G3"/>
-    <mergeCell ref="I2:J2"/>
-    <mergeCell ref="L3:M3"/>
+    <mergeCell ref="R7:S7"/>
+    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="G7:H7"/>
+    <mergeCell ref="D7:E7"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="C8:D8"/>
+    <mergeCell ref="E8:F8"/>
+    <mergeCell ref="G8:H8"/>
+    <mergeCell ref="G9:H9"/>
+    <mergeCell ref="D9:E9"/>
+    <mergeCell ref="V6:W6"/>
+    <mergeCell ref="Z6:AA6"/>
+    <mergeCell ref="Y4:Z4"/>
+    <mergeCell ref="AA4:AB4"/>
+    <mergeCell ref="Y5:Z5"/>
+    <mergeCell ref="AA5:AB5"/>
+    <mergeCell ref="V1:W1"/>
+    <mergeCell ref="V2:W2"/>
+    <mergeCell ref="U3:V3"/>
+    <mergeCell ref="W3:X3"/>
+    <mergeCell ref="Z2:AA2"/>
+    <mergeCell ref="Y3:Z3"/>
+    <mergeCell ref="AA3:AB3"/>
+    <mergeCell ref="AH1:AI1"/>
+    <mergeCell ref="AD2:AE2"/>
+    <mergeCell ref="AC3:AD3"/>
+    <mergeCell ref="AE3:AF3"/>
+    <mergeCell ref="AE5:AF5"/>
+    <mergeCell ref="AC5:AD5"/>
+    <mergeCell ref="S5:T5"/>
+    <mergeCell ref="U4:V4"/>
+    <mergeCell ref="W4:X4"/>
+    <mergeCell ref="U5:V5"/>
+    <mergeCell ref="W5:X5"/>
+    <mergeCell ref="AD6:AE6"/>
+    <mergeCell ref="AG2:AH2"/>
+    <mergeCell ref="AG4:AH4"/>
+    <mergeCell ref="AK2:AL2"/>
+    <mergeCell ref="AI4:AJ4"/>
+    <mergeCell ref="AK3:AL3"/>
+    <mergeCell ref="AM4:AN4"/>
+    <mergeCell ref="AI6:AJ6"/>
+    <mergeCell ref="AM6:AN6"/>
+    <mergeCell ref="AK5:AL5"/>
+    <mergeCell ref="AP1:AQ1"/>
+    <mergeCell ref="AV1:AW1"/>
+    <mergeCell ref="AP4:AQ4"/>
+    <mergeCell ref="AV4:AW4"/>
+    <mergeCell ref="AQ2:AR2"/>
+    <mergeCell ref="AO2:AP2"/>
+    <mergeCell ref="AO3:AP3"/>
+    <mergeCell ref="AQ3:AR3"/>
+    <mergeCell ref="AU2:AV2"/>
+    <mergeCell ref="AW2:AX2"/>
+    <mergeCell ref="AU3:AV3"/>
+    <mergeCell ref="AW3:AX3"/>
+    <mergeCell ref="AS2:AT2"/>
+    <mergeCell ref="AS3:AT3"/>
+    <mergeCell ref="AQ5:AR5"/>
+    <mergeCell ref="AU5:AV5"/>
+    <mergeCell ref="AW5:AX5"/>
+    <mergeCell ref="AS4:AT4"/>
+    <mergeCell ref="AV6:AW6"/>
+    <mergeCell ref="AP6:AQ6"/>
+    <mergeCell ref="AH7:AI7"/>
+    <mergeCell ref="AK4:AL4"/>
+    <mergeCell ref="AK6:AL6"/>
+    <mergeCell ref="AO5:AP5"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
@@ -2131,7 +2357,7 @@
       <selection activeCell="D24" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="1" width="39.140625" customWidth="1"/>
     <col min="2" max="2" width="38.140625" customWidth="1"/>
@@ -15462,7 +15688,7 @@
   <sheetViews>
     <sheetView workbookViewId="0"/>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>